<commit_message>
test the transform_casrec details
</commit_message>
<xml_diff>
--- a/tests/test_data/test_mapping_doc.xlsx
+++ b/tests/test_data/test_mapping_doc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration/docs/support_scripts/mapping_doc_to_json/tests/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration-mappings/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7A767F-4873-254A-B652-F705BC8E4FD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85951196-5A0F-C644-B1B9-8F82B0CD2ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20780" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{4D538E3F-ACC6-104C-8DE7-B6CEDF85F0BD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>table_name</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>status(blue)</t>
+  </si>
+  <si>
+    <t>conditional_lookup</t>
   </si>
 </sst>
 </file>
@@ -559,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EC6E68-D477-9249-8044-00C8897861C6}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,6 +793,32 @@
         <v>35</v>
       </c>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
format conditional lookups oops
</commit_message>
<xml_diff>
--- a/tests/test_data/test_mapping_doc.xlsx
+++ b/tests/test_data/test_mapping_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration-mappings/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85951196-5A0F-C644-B1B9-8F82B0CD2ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B09605-80D0-CA48-AFD5-B060251B94C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20780" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{4D538E3F-ACC6-104C-8DE7-B6CEDF85F0BD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>table_name</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>conditional_lookup</t>
+  </si>
+  <si>
+    <t>normal_lookup</t>
+  </si>
+  <si>
+    <t>I_a_lookup</t>
   </si>
 </sst>
 </file>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EC6E68-D477-9249-8044-00C8897861C6}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,6 +825,26 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add 'additional columns' to transform - better way of doing conditional lookups
</commit_message>
<xml_diff>
--- a/tests/test_data/test_mapping_doc.xlsx
+++ b/tests/test_data/test_mapping_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration-mappings/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C672346-40A2-9647-9C61-C00617B646A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A508954A-4401-3948-8A52-2834EA89408A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20780" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{4D538E3F-ACC6-104C-8DE7-B6CEDF85F0BD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>table_name</t>
   </si>
@@ -146,29 +146,36 @@
     <t>status</t>
   </si>
   <si>
-    <t>status(blue)</t>
-  </si>
-  <si>
     <t>conditional_lookup</t>
   </si>
   <si>
     <t>normal_lookup</t>
   </si>
   <si>
-    <t>I_a_lookup</t>
-  </si>
-  <si>
     <t>updated_date</t>
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>additional_columns</t>
+  </si>
+  <si>
+    <t>status_lookup</t>
+  </si>
+  <si>
+    <t>I_am_lookup</t>
+  </si>
+  <si>
+    <t>blue
+orange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +200,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -265,6 +277,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,15 +595,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EC6E68-D477-9249-8044-00C8897861C6}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,14 +643,17 @@
       <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -659,12 +677,13 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="7"/>
-      <c r="N2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N2" s="7"/>
+      <c r="O2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -681,11 +700,11 @@
       <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -701,11 +720,11 @@
       <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -721,11 +740,11 @@
       <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -741,11 +760,11 @@
       <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -761,11 +780,11 @@
       <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -781,11 +800,11 @@
       <c r="I8" t="s">
         <v>33</v>
       </c>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -801,11 +820,11 @@
       <c r="I9" t="s">
         <v>34</v>
       </c>
-      <c r="N9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -822,21 +841,24 @@
         <v>34</v>
       </c>
       <c r="J10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
-      </c>
-      <c r="K10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -848,27 +870,27 @@
         <v>17</v>
       </c>
       <c r="K11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="N11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
       <c r="G12" t="s">
         <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>